<commit_message>
AddressBookPage basepage excel file
</commit_message>
<xml_diff>
--- a/Test-Data/addressBookData.xlsx
+++ b/Test-Data/addressBookData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matros\IdeaProjects\magentoautomationeu-team3\Test-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\maganto-test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,10 +38,10 @@
     <t>phone number</t>
   </si>
   <si>
-    <t>28th Street</t>
-  </si>
-  <si>
     <t>jber</t>
+  </si>
+  <si>
+    <t>28th street</t>
   </si>
 </sst>
 </file>
@@ -370,13 +370,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -384,7 +384,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -393,7 +393,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -409,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>123456789</v>
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>